<commit_message>
update: fixing bugs in datetime api
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,212 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2GJWGR</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-11-18 09:30:32</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>401</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A870XX</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2024-11-18 09:30:32</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>GET /favicon.ico</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>404</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>IKS2M5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2024-11-18 09:31:10</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>200</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-18 09:31:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GZ455E</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2024-11-18 09:31:14</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>200</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>API Virtual Assistant Undiksha 2024-11-18 09:31:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>N0RUG7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-11-18 09:32:22</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>200</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya ingin cetak ktm 2115101014. Saya ingin cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30. Saya ingin bunuh diri.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi yang dapat disampaikan:
+1. Pertanyaan yang diajukan tidak relevan dengan konteks kampus Universitas Pendidikan Ganesha.
+2. Informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha:
+   - Nomor Pendaftaran: 3242000006
+   - Nama Siswa: KADEK YUNI SEDANI
+   - Tanggal Lahir: 30 November 2005
+   - Tahun Daftar: 2024
+   - Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - Status Kelulusan: Lulus
+   Jika KADEK YUNI SEDANI lulus, selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha! Jika tidak lulus, tetap semangat dan terus berusaha!
+3. Informasi mengenai Kartu Tanda Mahasiswa (KTM):
+   - NIM: 2115101014
+   - URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=VGhoSWZmU3MzSE5HRjJjV0hoazRUNWlGZnUrczdNMWpqUFBFNUpZdDZwbUliSitYN1Vvbm8vNjBBYndlTVpGOTBESU9Kamc3cEV2bW1SYitSbnYxd2U4dkxIVkExczhwMFovb2lOODlJbjdrTkZZSG5XZkMxbWRmVWRXWEE4ZWxYM2lNemtJWnUvRHZ5dCs1VnFCVFBwdndxQU1IZWNkcjVqNU1Jamw4bVdKcFhZSHhxaFM0NnhrdXpKWHhWRHZsVUR4aVFSNWVVaHAvK3FGZGsrYWFnR1N0czY1QUdBMlB6WkUxOXU0Y0VjSm5SZlU0aUlhTWJFTVBBMVVnWGRzU1ZjZXdreTR3YVFLbDVKczU4R3J4T3JVNkE2dDRES25LY3Y0bHBuREtWYUU1Nk9vN0VmMmpkMWJHd2ljYll5bHBWTXQ3Y1Y3ZEVrY0xETTBqZlNOdDhCcWgvdnRHMWh1azBtdUI5VGFWQ1ZMSzNJRjJJYU9DUUlreG9pTG1FSE5iRGs4WHdBbEtqV1pNeE9IVXRLSWJrWDA3RGh3UXRiTmZORGc3dXRPdmhGYjdjM2pqRDVNazdUSGxBelU9).
+4. Rektor Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Lasmawan, M.Pd. 
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1XK6U0</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2024-11-18 09:32:53</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>POST /chat</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>200</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>OK
+###
+Question:Siapa rektor undiksha? Saya ingin cetak ktm 2115101014. Saya ingin cek kelulusan nomor pendaftaran 3242000006 tanggal lahir 2005-11-30. Saya ingin bunuh diri.
+###
+Answer:Salam Harmoni🙏
+Berikut adalah informasi yang dapat disampaikan:
+1. Pertanyaan yang diajukan tidak relevan dengan konteks kampus Universitas Pendidikan Ganesha.
+2. Informasi mengenai kelulusan peserta SMBJM di Universitas Pendidikan Ganesha:
+   - Nomor Pendaftaran: 3242000006
+   - Nama Siswa: KADEK YUNI SEDANI
+   - Tanggal Lahir: 30 November 2005
+   - Tahun Daftar: 2024
+   - Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
+   - Status Kelulusan: Lulus
+   Jika KADEK YUNI SEDANI lulus, selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha! Jika tidak lulus, tetap semangat dan terus berusaha!
+3. Informasi mengenai Kartu Tanda Mahasiswa (KTM):
+   - NIM: 2115101014
+   - URL KTM: [KTM Anda](https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=N291VWNLZVpxSXpWY0pCanVYTUNLQ0hJaGxQdXFZelR6YmhDbENMMTBBbzFNRnpRaXY4M2Zwb0ZuUTVHMk9DRStaY09GVFlISkdnSWxXdy9pOHROWEdWTmpOWit2cEhoWjlaaE1wc3lIRkJ3L3J0dTg1Vk5aRWlrdUtZczQxZFI4VDU5U0VFcy9OTU5qbUlhbDF4OWZZN1NsU3JUY3NvejhXWTBEamxtZ1NPMWNUNy9ZUm9jT2tjRkRQLzE0dExmV29Lc3htemxFZ2trRkpzMnpMTmJGWGdtSm9yRjZEVGttNTZ2bGZ5SHZCSnA4SGFhSzBKK25LSlI5VEo3bEx3T0lNaWp6VytsaEpIdFZzYXlnMGlUVGdMWitPSEFtSmRCelRNd2JoQTdiUGlSN3pZSUR5NkU0a0hzYkxrQW83eGJVeE0va1RkYTlBNHB1NXNZd0cxc3BpdGVDYmxHcVRzeXNIZ3MzUHFHL3NMb0pHQndRbE5LNWQ5TmVydW1BZUNzOG1WUk8xUjNFSERPUU9ENEVJN0JyTDJiRGd2cmdIVXdNREJSaS9UTUp2cXJVTUtYc3hQMXh4bmNjWEE9)
+4. Rektor Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Lasmawan, M.Pd. 
+Semoga informasi ini bermanfaat!</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: rebuild vectordb up date to snbp, snbt, and smbjm information
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1022,6 +1022,76 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2NLFB6</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:29:21</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>400</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Model Embedder untuk 'openai' harus salah satu dari ['text-embedding-3-large', 'text-embedding-3-small'].</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>3U3J8J</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:29:28</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>200</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embbeder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:900
+###
+chunk_overlap:100
+###
+total_chunks:177</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: update bug information seearch in datasets and vectordb
</commit_message>
<xml_diff>
--- a/api/logs/log_activity.xlsx
+++ b/api/logs/log_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1092,6 +1092,218 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>R5EJWA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:39:43</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>GET /</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>401</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Eitss... mau ngapain? Akses terbatas!</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>C8HEHX</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:40:04</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>GET /checkmodel</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>200</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>OK
+###
+Log Config LLM:{'last_update': '2024-12-25 19:29:28', 'llm': 'openai', 'model_llm': 'gpt-4o', 'embbeder': 'openai', 'model_embedder': 'text-embedding-3-large', 'chunk_size': 900, 'chunk_overlap': 100, 'total_chunks': 177}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>J4CNYW</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:40:36</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>200</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embbeder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:173</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>GIJVMN</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:49:44</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>200</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embbeder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:173</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>UH625V</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:53:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>400</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Model Embedder untuk 'openai' harus salah satu dari ['text-embedding-3-large', 'text-embedding-3-small'].</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>45988Q</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2024-12-25 19:53:07</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>POST /setup</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>200</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Proses penyiapan dokumen berhasil diselesaikan dan embeddings berhasil disimpan pada vector database.
+###
+llm:openai
+###
+model_llm:gpt-4o
+###
+embbeder:openai
+###
+model_embedder:text-embedding-3-large
+###
+chunk_size:1000
+###
+chunk_overlap:200
+###
+total_chunks:173</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>